<commit_message>
Fix user and ficha assignment in app.py
</commit_message>
<xml_diff>
--- a/static/schedule-courses/Horario 1-2024 - 2559206.xlsx
+++ b/static/schedule-courses/Horario 1-2024 - 2559206.xlsx
@@ -66,7 +66,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -76,6 +76,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -471,7 +475,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:G25"/>
+  <dimension ref="A2:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,6 +520,16 @@
           <t>2559206</t>
         </is>
       </c>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>Instructor titular:</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>YEISON BARRIOS FUNIELES</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -692,7 +706,7 @@
       <c r="F11" s="3" t="inlineStr">
         <is>
           <t>Inglés 
- YORMAN ANDRÉS CALDERÓN YEPES 
+ NUEVO INGLÉS 
  705</t>
         </is>
       </c>
@@ -735,7 +749,7 @@
       <c r="F12" s="3" t="inlineStr">
         <is>
           <t>Inglés 
- YORMAN ANDRÉS CALDERÓN YEPES 
+ NUEVO INGLÉS 
  705</t>
         </is>
       </c>
@@ -966,6 +980,116 @@
       <c r="F25" s="4" t="n"/>
       <c r="G25" s="4" t="n"/>
     </row>
+    <row r="27">
+      <c r="A27" s="5" t="inlineStr">
+        <is>
+          <t>Palabra clave</t>
+        </is>
+      </c>
+      <c r="B27" s="5" t="inlineStr">
+        <is>
+          <t>Norma de Competencia (Sofíaplus)</t>
+        </is>
+      </c>
+      <c r="C27" s="5" t="inlineStr">
+        <is>
+          <t>Competencia</t>
+        </is>
+      </c>
+      <c r="D27" s="5" t="inlineStr">
+        <is>
+          <t>RAP</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="6" t="inlineStr">
+        <is>
+          <t>Pruebas</t>
+        </is>
+      </c>
+      <c r="B28" s="6" t="inlineStr">
+        <is>
+          <t>Desarrollar la solución de software de acuerdo con el diseño y metodologías de desarrollo.</t>
+        </is>
+      </c>
+      <c r="C28" s="6" t="inlineStr">
+        <is>
+          <t>Construcción del software.</t>
+        </is>
+      </c>
+      <c r="D28" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Realizar pruebas al software para verificar su funcionalidad.  </t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="6" t="inlineStr">
+        <is>
+          <t>Implantación + Manuales + Capacitación</t>
+        </is>
+      </c>
+      <c r="B29" s="6" t="inlineStr">
+        <is>
+          <t>Implementar la solución de software de acuerdo con los requisitos de operación y modelos de referencia.</t>
+        </is>
+      </c>
+      <c r="C29" s="6" t="inlineStr">
+        <is>
+          <t>Implantación del software.</t>
+        </is>
+      </c>
+      <c r="D29" s="6" t="inlineStr">
+        <is>
+          <t>Implantar el software de acuerdo con los niveles de servicio establecidos con el cliente.</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="6" t="inlineStr">
+        <is>
+          <t>Proyecto 2  + Manual Técnico</t>
+        </is>
+      </c>
+      <c r="B30" s="6" t="inlineStr">
+        <is>
+          <t>Implementar la solución de software de acuerdo con los requisitos de operación y modelos de referencia.</t>
+        </is>
+      </c>
+      <c r="C30" s="6" t="inlineStr">
+        <is>
+          <t>Implantación del software.</t>
+        </is>
+      </c>
+      <c r="D30" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Planear actividades de implantación del software de acuerdo con las condiciones del sistema. </t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="6" t="inlineStr">
+        <is>
+          <t>Calidad 3</t>
+        </is>
+      </c>
+      <c r="B31" s="6" t="inlineStr">
+        <is>
+          <t>Controlar la calidad del servicio de software de acuerdo con los estándares técnicos.</t>
+        </is>
+      </c>
+      <c r="C31" s="6" t="inlineStr">
+        <is>
+          <t>Adopción de buenas prácticas en el proceso de desarrollo de software.</t>
+        </is>
+      </c>
+      <c r="D31" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Realizar actividades de mejora de la calidad del software a partir de los resultados de la verificación.  </t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>